<commit_message>
refactoring and mass runs
</commit_message>
<xml_diff>
--- a/all_ml.xlsx
+++ b/all_ml.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymch\Desktop\ATLAS\ATLAS-L1-Trigger-Y4-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymch\OneDrive - University of Birmingham\Desktop\ATLAS\ATLAS-L1-Trigger-Y4-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF2633E-7CE9-42F8-AE4B-3C93A180356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5641F34C-225E-457E-96EC-CD1FC385C404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="43300" windowHeight="17531" xr2:uid="{E2FB39C9-4A23-4528-AACD-E809D9187880}"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="21738" windowHeight="17405" xr2:uid="{E2FB39C9-4A23-4528-AACD-E809D9187880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="83">
   <si>
     <t>AdaBoostClassifier</t>
   </si>
@@ -255,6 +255,36 @@
   </si>
   <si>
     <t>XGBClassifier</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Accuracy4</t>
+  </si>
+  <si>
+    <t>TN5</t>
+  </si>
+  <si>
+    <t>FP6</t>
+  </si>
+  <si>
+    <t>FN7</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>MSE9</t>
+  </si>
+  <si>
+    <t>Topo</t>
   </si>
 </sst>
 </file>
@@ -456,25 +486,25 @@
               <c:strCache>
                 <c:ptCount val="43"/>
                 <c:pt idx="0">
+                  <c:v>CategoricalNB</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>ClassifierChain</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>GaussianProcessClassifier</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>LabelPropagation</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>LabelSpreading</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>RadiusNeighborsClassifier</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MultiOutputClassifier</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>CategoricalNB</c:v>
+                  <c:v>RadiusNeighborsClassifier</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>ExtraTreesClassifier</c:v>
@@ -510,25 +540,25 @@
                   <c:v>SGDClassifier</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>OutputCodeClassifier</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>FixedThresholdClassifier</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>LogisticRegression</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>OneVsOneClassifier</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>OneVsRestClassifier</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>OutputCodeClassifier</c:v>
-                </c:pt>
                 <c:pt idx="23">
+                  <c:v>CalibratedClassifierCV</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>TunedThresholdClassifierCV</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>CalibratedClassifierCV</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>LinearSVC</c:v>
@@ -558,10 +588,10 @@
                   <c:v>LinearDiscriminantAnalysis</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>RidgeClassifierCV</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>RidgeClassifier</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>RidgeClassifierCV</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>NearestCentroid</c:v>
@@ -952,26 +982,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1260" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1307,10 +1317,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2146,12 +2152,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="24">
-  <a:schemeClr val="accent4"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="24">
   <a:schemeClr val="accent4"/>
 </cs:colorStyle>
@@ -3167,525 +3167,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>159026</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>119270</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>333954</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>159027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>87465</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>182879</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>349858</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>31804</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3712,16 +3207,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>970058</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>79513</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>238538</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>79514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>151074</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>166977</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>71561</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>166978</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3748,16 +3243,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>214685</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>39756</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>405517</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>135172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>278296</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>166978</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>79514</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>71562</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3788,12 +3283,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89490792-2E21-4B07-B492-5B60F58665E4}" name="Table2" displayName="Table2" ref="B3:W46" totalsRowShown="0">
-  <autoFilter ref="B3:W46" xr:uid="{89490792-2E21-4B07-B492-5B60F58665E4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:W46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89490792-2E21-4B07-B492-5B60F58665E4}" name="Table2" displayName="Table2" ref="B3:AF46" totalsRowShown="0">
+  <autoFilter ref="B3:AF46" xr:uid="{89490792-2E21-4B07-B492-5B60F58665E4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:AF46">
     <sortCondition descending="1" ref="C3:C46"/>
   </sortState>
-  <tableColumns count="22">
+  <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{EFFE131B-1FFA-47B7-A821-5574CBD2592C}" name="ML Algorithm"/>
     <tableColumn id="2" xr3:uid="{F73DCCCB-8B63-40C9-A391-AB2462111BB6}" name="Accuracy" dataDxfId="4"/>
     <tableColumn id="18" xr3:uid="{146333EC-3C75-4A47-95EA-BF3DDA5AF47B}" name="MSE" dataDxfId="3"/>
@@ -3822,6 +3317,15 @@
     <tableColumn id="14" xr3:uid="{8D3F5FE8-A024-4717-ACE5-613C3C892BCD}" name="FP3"/>
     <tableColumn id="15" xr3:uid="{9A6F061E-C05D-49D4-9264-B65EE6611C08}" name="FN3"/>
     <tableColumn id="16" xr3:uid="{06F3F3D9-73A1-4578-AB28-0B7AF3FB1F11}" name="TP3"/>
+    <tableColumn id="17" xr3:uid="{2747B920-72F6-4DE2-821E-4D075BA764AE}" name="Accuracy4"/>
+    <tableColumn id="20" xr3:uid="{2D03BB49-EF85-4E8B-AF01-9025B1EE3644}" name="TN5"/>
+    <tableColumn id="25" xr3:uid="{5CD8A061-241D-46BA-A24F-28DDFF67DAA6}" name="FP6"/>
+    <tableColumn id="26" xr3:uid="{6D54056E-F80D-41AB-ACD0-A8A745299772}" name="FN7"/>
+    <tableColumn id="27" xr3:uid="{A5C7BF97-1F32-486A-85BA-FD0969679BF3}" name="TP8"/>
+    <tableColumn id="28" xr3:uid="{D1FB5260-5613-43FE-90D3-E49909B762E8}" name="Precision"/>
+    <tableColumn id="29" xr3:uid="{D19D3423-F260-49BD-9F7E-E11F17E9F207}" name="Recall"/>
+    <tableColumn id="30" xr3:uid="{F64F23EB-35EC-492A-B7C4-222A86D1DF95}" name="F1"/>
+    <tableColumn id="31" xr3:uid="{A925A171-8A8E-4D0C-8AA0-B7A56CD6CE2D}" name="MSE9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4144,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C1DA7B-14B3-4B4E-8744-FCF5DDA7F499}">
-  <dimension ref="B1:W46"/>
+  <dimension ref="B1:AF46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V39" sqref="V39"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4162,7 +3666,7 @@
     <col min="16" max="18" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.3">
       <c r="M1" t="s">
         <v>70</v>
       </c>
@@ -4176,7 +3680,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -4186,8 +3690,11 @@
       <c r="Q2" t="s">
         <v>37</v>
       </c>
+      <c r="X2" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>45</v>
       </c>
@@ -4254,10 +3761,37 @@
       <c r="W3" t="s">
         <v>44</v>
       </c>
+      <c r="X3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -4281,27 +3815,27 @@
       <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" t="e">
+      <c r="J4">
+        <v>0.945260058031267</v>
+      </c>
+      <c r="K4">
+        <v>5.47399419687324E-2</v>
+      </c>
+      <c r="L4">
         <f>(Table2[[#This Row],[TP2]]/(Table2[[#This Row],[TP2]]+Table2[[#This Row],[FN2]]))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P4" t="s">
-        <v>38</v>
+        <v>0.94673343956294109</v>
+      </c>
+      <c r="M4">
+        <v>27018</v>
+      </c>
+      <c r="N4">
+        <v>1592</v>
+      </c>
+      <c r="O4">
+        <v>936</v>
+      </c>
+      <c r="P4">
+        <v>16636</v>
       </c>
       <c r="Q4" t="s">
         <v>38</v>
@@ -4325,10 +3859,37 @@
       <c r="W4" t="s">
         <v>38</v>
       </c>
+      <c r="X4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -4396,10 +3957,37 @@
       <c r="W5" t="s">
         <v>38</v>
       </c>
+      <c r="X5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -4467,10 +4055,37 @@
       <c r="W6" t="s">
         <v>38</v>
       </c>
+      <c r="X6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -4538,10 +4153,37 @@
       <c r="W7" t="s">
         <v>38</v>
       </c>
+      <c r="X7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -4609,8 +4251,35 @@
       <c r="W8" t="s">
         <v>38</v>
       </c>
+      <c r="X8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -4680,10 +4349,37 @@
       <c r="W9" t="s">
         <v>38</v>
       </c>
+      <c r="X9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -4707,27 +4403,27 @@
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10">
-        <v>0.945260058031267</v>
-      </c>
-      <c r="K10">
-        <v>5.47399419687324E-2</v>
-      </c>
-      <c r="L10">
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" t="e">
         <f>(Table2[[#This Row],[TP2]]/(Table2[[#This Row],[TP2]]+Table2[[#This Row],[FN2]]))</f>
-        <v>0.94673343956294109</v>
-      </c>
-      <c r="M10">
-        <v>27018</v>
-      </c>
-      <c r="N10">
-        <v>1592</v>
-      </c>
-      <c r="O10">
-        <v>936</v>
-      </c>
-      <c r="P10">
-        <v>16636</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" t="s">
+        <v>38</v>
       </c>
       <c r="Q10" t="s">
         <v>38</v>
@@ -4751,8 +4447,35 @@
       <c r="W10" t="s">
         <v>38</v>
       </c>
+      <c r="X10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -4822,8 +4545,35 @@
       <c r="W11">
         <v>17258</v>
       </c>
+      <c r="X11">
+        <v>0.97265356952245396</v>
+      </c>
+      <c r="Y11">
+        <v>2618</v>
+      </c>
+      <c r="Z11">
+        <v>1734</v>
+      </c>
+      <c r="AA11">
+        <v>418</v>
+      </c>
+      <c r="AB11">
+        <v>73924</v>
+      </c>
+      <c r="AC11">
+        <v>0.97708107536545996</v>
+      </c>
+      <c r="AD11">
+        <v>0.99437733717145005</v>
+      </c>
+      <c r="AE11">
+        <v>0.98565333333333305</v>
+      </c>
+      <c r="AF11">
+        <v>2.73464304775459E-2</v>
+      </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>72</v>
       </c>
@@ -4893,8 +4643,35 @@
       <c r="W12">
         <v>17045</v>
       </c>
+      <c r="X12">
+        <v>0.97283147380994694</v>
+      </c>
+      <c r="Y12">
+        <v>2636</v>
+      </c>
+      <c r="Z12">
+        <v>1716</v>
+      </c>
+      <c r="AA12">
+        <v>422</v>
+      </c>
+      <c r="AB12">
+        <v>73920</v>
+      </c>
+      <c r="AC12">
+        <v>0.97731239092495603</v>
+      </c>
+      <c r="AD12">
+        <v>0.99432353178553101</v>
+      </c>
+      <c r="AE12">
+        <v>0.98574457587112696</v>
+      </c>
+      <c r="AF12">
+        <v>2.7168526190052601E-2</v>
+      </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -4964,8 +4741,35 @@
       <c r="W13">
         <v>17020</v>
       </c>
+      <c r="X13">
+        <v>0.965753424657534</v>
+      </c>
+      <c r="Y13">
+        <v>1747</v>
+      </c>
+      <c r="Z13">
+        <v>2605</v>
+      </c>
+      <c r="AA13">
+        <v>90</v>
+      </c>
+      <c r="AB13">
+        <v>74252</v>
+      </c>
+      <c r="AC13">
+        <v>0.96610588495517602</v>
+      </c>
+      <c r="AD13">
+        <v>0.99878937881681895</v>
+      </c>
+      <c r="AE13">
+        <v>0.98217580804105797</v>
+      </c>
+      <c r="AF13">
+        <v>3.4246575342465703E-2</v>
+      </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -5035,8 +4839,35 @@
       <c r="W14">
         <v>17126</v>
       </c>
+      <c r="X14">
+        <v>0.97260273972602695</v>
+      </c>
+      <c r="Y14">
+        <v>2643</v>
+      </c>
+      <c r="Z14">
+        <v>1709</v>
+      </c>
+      <c r="AA14">
+        <v>447</v>
+      </c>
+      <c r="AB14">
+        <v>73895</v>
+      </c>
+      <c r="AC14">
+        <v>0.97739537590603598</v>
+      </c>
+      <c r="AD14">
+        <v>0.993987248123537</v>
+      </c>
+      <c r="AE14">
+        <v>0.98562149040321101</v>
+      </c>
+      <c r="AF14">
+        <v>2.7397260273972601E-2</v>
+      </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -5106,8 +4937,35 @@
       <c r="W15">
         <v>17117</v>
       </c>
+      <c r="X15">
+        <v>0.97342872391795998</v>
+      </c>
+      <c r="Y15">
+        <v>2679</v>
+      </c>
+      <c r="Z15">
+        <v>1673</v>
+      </c>
+      <c r="AA15">
+        <v>418</v>
+      </c>
+      <c r="AB15">
+        <v>73924</v>
+      </c>
+      <c r="AC15">
+        <v>0.97786949217561503</v>
+      </c>
+      <c r="AD15">
+        <v>0.99437733717145005</v>
+      </c>
+      <c r="AE15">
+        <v>0.98605432876036203</v>
+      </c>
+      <c r="AF15">
+        <v>2.65712760820392E-2</v>
+      </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -5177,8 +5035,35 @@
       <c r="W16">
         <v>17194</v>
       </c>
+      <c r="X16">
+        <v>0.97259003227691998</v>
+      </c>
+      <c r="Y16">
+        <v>2377</v>
+      </c>
+      <c r="Z16">
+        <v>1975</v>
+      </c>
+      <c r="AA16">
+        <v>182</v>
+      </c>
+      <c r="AB16">
+        <v>74160</v>
+      </c>
+      <c r="AC16">
+        <v>0.97405923688185403</v>
+      </c>
+      <c r="AD16">
+        <v>0.99755185494067899</v>
+      </c>
+      <c r="AE16">
+        <v>0.98566558344464605</v>
+      </c>
+      <c r="AF16">
+        <v>2.7409967723079201E-2</v>
+      </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>64</v>
       </c>
@@ -5248,8 +5133,35 @@
       <c r="W17">
         <v>16054</v>
       </c>
+      <c r="X17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -5319,8 +5231,35 @@
       <c r="W18">
         <v>16657</v>
       </c>
+      <c r="X18">
+        <v>0.97082369685109404</v>
+      </c>
+      <c r="Y18">
+        <v>2719</v>
+      </c>
+      <c r="Z18">
+        <v>1633</v>
+      </c>
+      <c r="AA18">
+        <v>663</v>
+      </c>
+      <c r="AB18">
+        <v>73679</v>
+      </c>
+      <c r="AC18">
+        <v>0.97831686849373201</v>
+      </c>
+      <c r="AD18">
+        <v>0.99108175728390402</v>
+      </c>
+      <c r="AE18">
+        <v>0.98465794432490905</v>
+      </c>
+      <c r="AF18">
+        <v>2.9176303148905802E-2</v>
+      </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>27</v>
       </c>
@@ -5390,8 +5329,35 @@
       <c r="W19">
         <v>16338</v>
       </c>
+      <c r="X19">
+        <v>0.97299667064833395</v>
+      </c>
+      <c r="Y19">
+        <v>2602</v>
+      </c>
+      <c r="Z19">
+        <v>1750</v>
+      </c>
+      <c r="AA19">
+        <v>375</v>
+      </c>
+      <c r="AB19">
+        <v>73967</v>
+      </c>
+      <c r="AC19">
+        <v>0.97688762100981197</v>
+      </c>
+      <c r="AD19">
+        <v>0.994955745070081</v>
+      </c>
+      <c r="AE19">
+        <v>0.98583890336467594</v>
+      </c>
+      <c r="AF19">
+        <v>2.7003329351665901E-2</v>
+      </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -5461,8 +5427,35 @@
       <c r="W20">
         <v>16226</v>
       </c>
+      <c r="X20">
+        <v>0.96388542963885404</v>
+      </c>
+      <c r="Y20">
+        <v>1880</v>
+      </c>
+      <c r="Z20">
+        <v>2472</v>
+      </c>
+      <c r="AA20">
+        <v>370</v>
+      </c>
+      <c r="AB20">
+        <v>73972</v>
+      </c>
+      <c r="AC20">
+        <v>0.96766260268954996</v>
+      </c>
+      <c r="AD20">
+        <v>0.99502300180248004</v>
+      </c>
+      <c r="AE20">
+        <v>0.98115209634846701</v>
+      </c>
+      <c r="AF20">
+        <v>3.6114570361145702E-2</v>
+      </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -5532,10 +5525,37 @@
       <c r="W21">
         <v>15959</v>
       </c>
+      <c r="X21">
+        <v>0.93287925381858805</v>
+      </c>
+      <c r="Y21">
+        <v>914</v>
+      </c>
+      <c r="Z21">
+        <v>3438</v>
+      </c>
+      <c r="AA21">
+        <v>1844</v>
+      </c>
+      <c r="AB21">
+        <v>72498</v>
+      </c>
+      <c r="AC21">
+        <v>0.95472503160556199</v>
+      </c>
+      <c r="AD21">
+        <v>0.97519571709127995</v>
+      </c>
+      <c r="AE21">
+        <v>0.964851807982539</v>
+      </c>
+      <c r="AF21">
+        <v>6.7120746181411506E-2</v>
+      </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>0.94134078212290495</v>
@@ -5603,10 +5623,37 @@
       <c r="W22">
         <v>16220</v>
       </c>
+      <c r="X22" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>0.94134078212290495</v>
@@ -5674,10 +5721,37 @@
       <c r="W23">
         <v>16220</v>
       </c>
+      <c r="X23">
+        <v>0.96388542963885404</v>
+      </c>
+      <c r="Y23">
+        <v>1880</v>
+      </c>
+      <c r="Z23">
+        <v>2472</v>
+      </c>
+      <c r="AA23">
+        <v>370</v>
+      </c>
+      <c r="AB23">
+        <v>73972</v>
+      </c>
+      <c r="AC23">
+        <v>0.96766260268954996</v>
+      </c>
+      <c r="AD23">
+        <v>0.99502300180248004</v>
+      </c>
+      <c r="AE23">
+        <v>0.98115209634846701</v>
+      </c>
+      <c r="AF23">
+        <v>3.6114570361145702E-2</v>
+      </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>0.94134078212290495</v>
@@ -5745,10 +5819,37 @@
       <c r="W24">
         <v>16220</v>
       </c>
+      <c r="X24">
+        <v>0.96388542963885404</v>
+      </c>
+      <c r="Y24">
+        <v>1880</v>
+      </c>
+      <c r="Z24">
+        <v>2472</v>
+      </c>
+      <c r="AA24">
+        <v>370</v>
+      </c>
+      <c r="AB24">
+        <v>73972</v>
+      </c>
+      <c r="AC24">
+        <v>0.96766260268954996</v>
+      </c>
+      <c r="AD24">
+        <v>0.99502300180248004</v>
+      </c>
+      <c r="AE24">
+        <v>0.98115209634846701</v>
+      </c>
+      <c r="AF24">
+        <v>3.6114570361145702E-2</v>
+      </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25">
         <v>0.94134078212290495</v>
@@ -5816,10 +5917,37 @@
       <c r="W25">
         <v>16220</v>
       </c>
+      <c r="X25">
+        <v>0.96388542963885404</v>
+      </c>
+      <c r="Y25">
+        <v>1880</v>
+      </c>
+      <c r="Z25">
+        <v>2472</v>
+      </c>
+      <c r="AA25">
+        <v>370</v>
+      </c>
+      <c r="AB25">
+        <v>73972</v>
+      </c>
+      <c r="AC25">
+        <v>0.96766260268954996</v>
+      </c>
+      <c r="AD25">
+        <v>0.99502300180248004</v>
+      </c>
+      <c r="AE25">
+        <v>0.98115209634846701</v>
+      </c>
+      <c r="AF25">
+        <v>3.6114570361145702E-2</v>
+      </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26">
         <v>0.94134078212290495</v>
@@ -5887,10 +6015,37 @@
       <c r="W26">
         <v>16220</v>
       </c>
+      <c r="X26">
+        <v>0.96388542963885404</v>
+      </c>
+      <c r="Y26">
+        <v>1880</v>
+      </c>
+      <c r="Z26">
+        <v>2472</v>
+      </c>
+      <c r="AA26">
+        <v>370</v>
+      </c>
+      <c r="AB26">
+        <v>73972</v>
+      </c>
+      <c r="AC26">
+        <v>0.96766260268954996</v>
+      </c>
+      <c r="AD26">
+        <v>0.99502300180248004</v>
+      </c>
+      <c r="AE26">
+        <v>0.98115209634846701</v>
+      </c>
+      <c r="AF26">
+        <v>3.6114570361145702E-2</v>
+      </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>0.94099432679398898</v>
@@ -5900,68 +6055,95 @@
       </c>
       <c r="E27">
         <f>(Table2[[#This Row],[TP]]/(Table2[[#This Row],[TP]]+Table2[[#This Row],[FN]]))</f>
-        <v>0.96648076485317547</v>
+        <v>0.93842476667425445</v>
       </c>
       <c r="F27">
-        <v>26474</v>
+        <v>26967</v>
       </c>
       <c r="G27">
-        <v>2136</v>
+        <v>1643</v>
       </c>
       <c r="H27">
-        <v>589</v>
+        <v>1082</v>
       </c>
       <c r="I27">
-        <v>16983</v>
+        <v>16490</v>
       </c>
       <c r="J27">
-        <v>0.94837815599151098</v>
+        <v>0.94872461132042696</v>
       </c>
       <c r="K27">
-        <v>5.1621844008488099E-2</v>
+        <v>5.1275388679572098E-2</v>
       </c>
       <c r="L27">
         <f>(Table2[[#This Row],[TP2]]/(Table2[[#This Row],[TP2]]+Table2[[#This Row],[FN2]]))</f>
-        <v>0.97735033007056682</v>
+        <v>0.94576599134987482</v>
       </c>
       <c r="M27">
-        <v>26624</v>
+        <v>27195</v>
       </c>
       <c r="N27">
-        <v>1986</v>
+        <v>1415</v>
       </c>
       <c r="O27">
-        <v>398</v>
+        <v>953</v>
       </c>
       <c r="P27">
-        <v>17174</v>
+        <v>16619</v>
       </c>
       <c r="Q27">
-        <v>0.93571088302801897</v>
+        <v>0.93343726993200804</v>
       </c>
       <c r="R27">
-        <v>6.4289116971980406E-2</v>
+        <v>6.6562730067991793E-2</v>
       </c>
       <c r="S27">
         <f>(Table2[[#This Row],[TP3]]/(Table2[[#This Row],[TP3]]+Table2[[#This Row],[FN3]]))</f>
-        <v>0.95777373093557938</v>
+        <v>0.92066924652856819</v>
       </c>
       <c r="T27">
-        <v>26383</v>
+        <v>26930</v>
       </c>
       <c r="U27">
-        <v>2227</v>
+        <v>1680</v>
       </c>
       <c r="V27">
-        <v>742</v>
+        <v>1394</v>
       </c>
       <c r="W27">
-        <v>16830</v>
+        <v>16178</v>
+      </c>
+      <c r="X27">
+        <v>0.94504028261366801</v>
+      </c>
+      <c r="Y27">
+        <v>32</v>
+      </c>
+      <c r="Z27">
+        <v>4320</v>
+      </c>
+      <c r="AA27">
+        <v>5</v>
+      </c>
+      <c r="AB27">
+        <v>74337</v>
+      </c>
+      <c r="AC27">
+        <v>0.94507799687249705</v>
+      </c>
+      <c r="AD27">
+        <v>0.99993274326760095</v>
+      </c>
+      <c r="AE27">
+        <v>0.97173184138458402</v>
+      </c>
+      <c r="AF27">
+        <v>5.4959717386331798E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C28">
         <v>0.94099432679398898</v>
@@ -5971,66 +6153,93 @@
       </c>
       <c r="E28">
         <f>(Table2[[#This Row],[TP]]/(Table2[[#This Row],[TP]]+Table2[[#This Row],[FN]]))</f>
-        <v>0.93842476667425445</v>
+        <v>0.96648076485317547</v>
       </c>
       <c r="F28">
-        <v>26967</v>
+        <v>26474</v>
       </c>
       <c r="G28">
-        <v>1643</v>
+        <v>2136</v>
       </c>
       <c r="H28">
-        <v>1082</v>
+        <v>589</v>
       </c>
       <c r="I28">
-        <v>16490</v>
+        <v>16983</v>
       </c>
       <c r="J28">
-        <v>0.94872461132042696</v>
+        <v>0.94837815599151098</v>
       </c>
       <c r="K28">
-        <v>5.1275388679572098E-2</v>
+        <v>5.1621844008488099E-2</v>
       </c>
       <c r="L28">
         <f>(Table2[[#This Row],[TP2]]/(Table2[[#This Row],[TP2]]+Table2[[#This Row],[FN2]]))</f>
-        <v>0.94576599134987482</v>
+        <v>0.97735033007056682</v>
       </c>
       <c r="M28">
-        <v>27195</v>
+        <v>26624</v>
       </c>
       <c r="N28">
-        <v>1415</v>
+        <v>1986</v>
       </c>
       <c r="O28">
-        <v>953</v>
+        <v>398</v>
       </c>
       <c r="P28">
-        <v>16619</v>
+        <v>17174</v>
       </c>
       <c r="Q28">
-        <v>0.93343726993200804</v>
+        <v>0.93571088302801897</v>
       </c>
       <c r="R28">
-        <v>6.6562730067991793E-2</v>
+        <v>6.4289116971980406E-2</v>
       </c>
       <c r="S28">
         <f>(Table2[[#This Row],[TP3]]/(Table2[[#This Row],[TP3]]+Table2[[#This Row],[FN3]]))</f>
-        <v>0.92066924652856819</v>
+        <v>0.95777373093557938</v>
       </c>
       <c r="T28">
-        <v>26930</v>
+        <v>26383</v>
       </c>
       <c r="U28">
-        <v>1680</v>
+        <v>2227</v>
       </c>
       <c r="V28">
-        <v>1394</v>
+        <v>742</v>
       </c>
       <c r="W28">
-        <v>16178</v>
+        <v>16830</v>
+      </c>
+      <c r="X28">
+        <v>0.88245609576333595</v>
+      </c>
+      <c r="Y28">
+        <v>3515</v>
+      </c>
+      <c r="Z28">
+        <v>837</v>
+      </c>
+      <c r="AA28">
+        <v>8413</v>
+      </c>
+      <c r="AB28">
+        <v>65929</v>
+      </c>
+      <c r="AC28">
+        <v>0.98746367911811395</v>
+      </c>
+      <c r="AD28">
+        <v>0.88683382206558803</v>
+      </c>
+      <c r="AE28">
+        <v>0.93444737364288299</v>
+      </c>
+      <c r="AF28">
+        <v>0.117543904236663</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -6100,8 +6309,35 @@
       <c r="W29">
         <v>16104</v>
       </c>
+      <c r="X29">
+        <v>0.93780974407197504</v>
+      </c>
+      <c r="Y29">
+        <v>207</v>
+      </c>
+      <c r="Z29">
+        <v>4145</v>
+      </c>
+      <c r="AA29">
+        <v>749</v>
+      </c>
+      <c r="AB29">
+        <v>73593</v>
+      </c>
+      <c r="AC29">
+        <v>0.94667987342097804</v>
+      </c>
+      <c r="AD29">
+        <v>0.98992494148664201</v>
+      </c>
+      <c r="AE29">
+        <v>0.96781956864807905</v>
+      </c>
+      <c r="AF29">
+        <v>6.2190255928024997E-2</v>
+      </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -6171,8 +6407,35 @@
       <c r="W30">
         <v>17217</v>
       </c>
+      <c r="X30">
+        <v>0.97168780339034699</v>
+      </c>
+      <c r="Y30">
+        <v>2566</v>
+      </c>
+      <c r="Z30">
+        <v>1786</v>
+      </c>
+      <c r="AA30">
+        <v>442</v>
+      </c>
+      <c r="AB30">
+        <v>73900</v>
+      </c>
+      <c r="AC30">
+        <v>0.97640250508680604</v>
+      </c>
+      <c r="AD30">
+        <v>0.99405450485593605</v>
+      </c>
+      <c r="AE30">
+        <v>0.98514943877142902</v>
+      </c>
+      <c r="AF30">
+        <v>2.83121966096525E-2</v>
+      </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -6242,8 +6505,35 @@
       <c r="W31">
         <v>16156</v>
       </c>
+      <c r="X31">
+        <v>0.95332553943121401</v>
+      </c>
+      <c r="Y31">
+        <v>2607</v>
+      </c>
+      <c r="Z31">
+        <v>1745</v>
+      </c>
+      <c r="AA31">
+        <v>1928</v>
+      </c>
+      <c r="AB31">
+        <v>72414</v>
+      </c>
+      <c r="AC31">
+        <v>0.97646947774376602</v>
+      </c>
+      <c r="AD31">
+        <v>0.97406580398697895</v>
+      </c>
+      <c r="AE31">
+        <v>0.97526615982383902</v>
+      </c>
+      <c r="AF31">
+        <v>4.6674460568785402E-2</v>
+      </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -6313,8 +6603,35 @@
       <c r="W32">
         <v>15660</v>
       </c>
+      <c r="X32">
+        <v>0.97065850001270704</v>
+      </c>
+      <c r="Y32">
+        <v>2398</v>
+      </c>
+      <c r="Z32">
+        <v>1954</v>
+      </c>
+      <c r="AA32">
+        <v>355</v>
+      </c>
+      <c r="AB32">
+        <v>73987</v>
+      </c>
+      <c r="AC32">
+        <v>0.97426949868977197</v>
+      </c>
+      <c r="AD32">
+        <v>0.99522477199967696</v>
+      </c>
+      <c r="AE32">
+        <v>0.98463565406599496</v>
+      </c>
+      <c r="AF32">
+        <v>2.9341499987292501E-2</v>
+      </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -6384,8 +6701,35 @@
       <c r="W33">
         <v>16102</v>
       </c>
+      <c r="X33">
+        <v>0.95255038503570699</v>
+      </c>
+      <c r="Y33">
+        <v>2508</v>
+      </c>
+      <c r="Z33">
+        <v>1844</v>
+      </c>
+      <c r="AA33">
+        <v>1890</v>
+      </c>
+      <c r="AB33">
+        <v>72452</v>
+      </c>
+      <c r="AC33">
+        <v>0.97518035964251104</v>
+      </c>
+      <c r="AD33">
+        <v>0.97457695515320997</v>
+      </c>
+      <c r="AE33">
+        <v>0.97487856402804096</v>
+      </c>
+      <c r="AF33">
+        <v>4.7449614964292001E-2</v>
+      </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -6455,8 +6799,35 @@
       <c r="W34">
         <v>8252</v>
       </c>
+      <c r="X34">
+        <v>0.937885988766615</v>
+      </c>
+      <c r="Y34">
+        <v>259</v>
+      </c>
+      <c r="Z34">
+        <v>4093</v>
+      </c>
+      <c r="AA34">
+        <v>795</v>
+      </c>
+      <c r="AB34">
+        <v>73547</v>
+      </c>
+      <c r="AC34">
+        <v>0.94728232869654805</v>
+      </c>
+      <c r="AD34">
+        <v>0.98930617954857203</v>
+      </c>
+      <c r="AE34">
+        <v>0.967838296640391</v>
+      </c>
+      <c r="AF34">
+        <v>6.2114011233385003E-2</v>
+      </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>10</v>
       </c>
@@ -6526,8 +6897,35 @@
       <c r="W35">
         <v>15325</v>
       </c>
+      <c r="X35" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>11</v>
       </c>
@@ -6597,8 +6995,35 @@
       <c r="W36">
         <v>8405</v>
       </c>
+      <c r="X36">
+        <v>0.93990647317457499</v>
+      </c>
+      <c r="Y36">
+        <v>179</v>
+      </c>
+      <c r="Z36">
+        <v>4173</v>
+      </c>
+      <c r="AA36">
+        <v>556</v>
+      </c>
+      <c r="AB36">
+        <v>73786</v>
+      </c>
+      <c r="AC36">
+        <v>0.94647186341538503</v>
+      </c>
+      <c r="AD36">
+        <v>0.99252105135724</v>
+      </c>
+      <c r="AE36">
+        <v>0.96894964576726295</v>
+      </c>
+      <c r="AF36">
+        <v>6.0093526825425E-2</v>
+      </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -6668,10 +7093,37 @@
       <c r="W37">
         <v>13975</v>
       </c>
+      <c r="X37">
+        <v>0.96392355198617397</v>
+      </c>
+      <c r="Y37">
+        <v>1979</v>
+      </c>
+      <c r="Z37">
+        <v>2373</v>
+      </c>
+      <c r="AA37">
+        <v>466</v>
+      </c>
+      <c r="AB37">
+        <v>73876</v>
+      </c>
+      <c r="AC37">
+        <v>0.96887828037088997</v>
+      </c>
+      <c r="AD37">
+        <v>0.99373167254042105</v>
+      </c>
+      <c r="AE37">
+        <v>0.98114761174306497</v>
+      </c>
+      <c r="AF37">
+        <v>3.6076448013825702E-2</v>
+      </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C38">
         <v>0.87778788272487096</v>
@@ -6739,10 +7191,37 @@
       <c r="W38">
         <v>13915</v>
       </c>
+      <c r="X38">
+        <v>0.95455816199456101</v>
+      </c>
+      <c r="Y38">
+        <v>841</v>
+      </c>
+      <c r="Z38">
+        <v>3511</v>
+      </c>
+      <c r="AA38">
+        <v>65</v>
+      </c>
+      <c r="AB38">
+        <v>74277</v>
+      </c>
+      <c r="AC38">
+        <v>0.95486450352239405</v>
+      </c>
+      <c r="AD38">
+        <v>0.99912566247881396</v>
+      </c>
+      <c r="AE38">
+        <v>0.97649378820745403</v>
+      </c>
+      <c r="AF38">
+        <v>4.5441838005438703E-2</v>
+      </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>0.87778788272487096</v>
@@ -6810,8 +7289,35 @@
       <c r="W39">
         <v>13915</v>
       </c>
+      <c r="X39">
+        <v>0.95434213535974699</v>
+      </c>
+      <c r="Y39">
+        <v>825</v>
+      </c>
+      <c r="Z39">
+        <v>3527</v>
+      </c>
+      <c r="AA39">
+        <v>66</v>
+      </c>
+      <c r="AB39">
+        <v>74276</v>
+      </c>
+      <c r="AC39">
+        <v>0.95466755780625401</v>
+      </c>
+      <c r="AD39">
+        <v>0.99911221113233395</v>
+      </c>
+      <c r="AE39">
+        <v>0.97638437017319002</v>
+      </c>
+      <c r="AF39">
+        <v>4.5657864640252101E-2</v>
+      </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>9</v>
       </c>
@@ -6881,8 +7387,35 @@
       <c r="W40">
         <v>14222</v>
       </c>
+      <c r="X40" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>8</v>
       </c>
@@ -6952,8 +7485,35 @@
       <c r="W41">
         <v>16669</v>
       </c>
+      <c r="X41" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>24</v>
       </c>
@@ -7023,8 +7583,35 @@
       <c r="W42">
         <v>16758</v>
       </c>
+      <c r="X42" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -7094,8 +7681,35 @@
       <c r="W43">
         <v>16752</v>
       </c>
+      <c r="X43">
+        <v>0.94160927135486805</v>
+      </c>
+      <c r="Y43">
+        <v>2293</v>
+      </c>
+      <c r="Z43">
+        <v>2059</v>
+      </c>
+      <c r="AA43">
+        <v>2536</v>
+      </c>
+      <c r="AB43">
+        <v>71806</v>
+      </c>
+      <c r="AC43">
+        <v>0.97212482231097197</v>
+      </c>
+      <c r="AD43">
+        <v>0.96588738532727103</v>
+      </c>
+      <c r="AE43">
+        <v>0.968996066312657</v>
+      </c>
+      <c r="AF43">
+        <v>5.8390728645131701E-2</v>
+      </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>29</v>
       </c>
@@ -7165,8 +7779,35 @@
       <c r="W44">
         <v>16743</v>
       </c>
+      <c r="X44">
+        <v>0.90644775967672198</v>
+      </c>
+      <c r="Y44">
+        <v>2016</v>
+      </c>
+      <c r="Z44">
+        <v>2336</v>
+      </c>
+      <c r="AA44">
+        <v>5026</v>
+      </c>
+      <c r="AB44">
+        <v>69316</v>
+      </c>
+      <c r="AC44">
+        <v>0.96739797912130798</v>
+      </c>
+      <c r="AD44">
+        <v>0.93239353259261204</v>
+      </c>
+      <c r="AE44">
+        <v>0.94957327013438897</v>
+      </c>
+      <c r="AF44">
+        <v>9.3552240323277497E-2</v>
+      </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>21</v>
       </c>
@@ -7236,8 +7877,35 @@
       <c r="W45">
         <v>15962</v>
       </c>
+      <c r="X45">
+        <v>0.94469718148778803</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>4352</v>
+      </c>
+      <c r="AA45">
+        <v>0</v>
+      </c>
+      <c r="AB45">
+        <v>74342</v>
+      </c>
+      <c r="AC45">
+        <v>0.94469718148778803</v>
+      </c>
+      <c r="AD45">
+        <v>1</v>
+      </c>
+      <c r="AE45">
+        <v>0.97156224679160397</v>
+      </c>
+      <c r="AF45">
+        <v>5.5302818512211797E-2</v>
+      </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>32</v>
       </c>
@@ -7306,11 +7974,86 @@
       </c>
       <c r="W46">
         <v>0</v>
+      </c>
+      <c r="X46">
+        <v>0.94469718148778803</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>4352</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46">
+        <v>74342</v>
+      </c>
+      <c r="AC46">
+        <v>0.94469718148778803</v>
+      </c>
+      <c r="AD46">
+        <v>1</v>
+      </c>
+      <c r="AE46">
+        <v>0.97156224679160397</v>
+      </c>
+      <c r="AF46">
+        <v>5.5302818512211797E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576 J1:J1048576 Q1:Q1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C46">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576 L1:L1048576 S1:S1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:X46">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -7322,20 +8065,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C46">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576 L1:L1048576 S1:S1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="AC4:AC46">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7346,8 +8077,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="AE4:AE46">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
please confirm old and new efex classifier results are same (inconsistencies(!), look at training on iso vs 99 behaviour for all classifiers (why only best performing classfiers prefer 99 supercells, but mid range classifiers prefer iso to 99, pareto optimisation still broken
</commit_message>
<xml_diff>
--- a/all_ml.xlsx
+++ b/all_ml.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymch\OneDrive - University of Birmingham\Desktop\ATLAS\ATLAS-L1-Trigger-Y4-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ATLAS-L1-Trigger-Y4-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5641F34C-225E-457E-96EC-CD1FC385C404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FBFDC-FD3D-40B9-AD86-D8CEE12CA206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="21738" windowHeight="17405" xr2:uid="{E2FB39C9-4A23-4528-AACD-E809D9187880}"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="21738" windowHeight="17405" tabRatio="599" xr2:uid="{E2FB39C9-4A23-4528-AACD-E809D9187880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="83">
   <si>
     <t>AdaBoostClassifier</t>
   </si>
@@ -306,15 +306,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -322,17 +328,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -3207,16 +3249,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>238538</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>79514</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>103366</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>127221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>71561</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>166977</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>166978</xdr:rowOff>
+      <xdr:rowOff>23854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3243,16 +3285,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>405517</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>135172</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>254442</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>143123</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>79514</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>71562</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>174930</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>79513</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3290,9 +3332,9 @@
   </sortState>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{EFFE131B-1FFA-47B7-A821-5574CBD2592C}" name="ML Algorithm"/>
-    <tableColumn id="2" xr3:uid="{F73DCCCB-8B63-40C9-A391-AB2462111BB6}" name="Accuracy" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{146333EC-3C75-4A47-95EA-BF3DDA5AF47B}" name="MSE" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{BC3E5747-ED6C-44AF-A29F-B26F11980C15}" name="Efficiency" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{F73DCCCB-8B63-40C9-A391-AB2462111BB6}" name="Accuracy" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{146333EC-3C75-4A47-95EA-BF3DDA5AF47B}" name="MSE" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{BC3E5747-ED6C-44AF-A29F-B26F11980C15}" name="Efficiency" dataDxfId="5">
       <calculatedColumnFormula>(Table2[[#This Row],[TP]]/(Table2[[#This Row],[TP]]+Table2[[#This Row],[FN]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{A1B31B55-CFD6-44D3-93CE-47F91D1A836D}" name="TN"/>
@@ -3301,7 +3343,7 @@
     <tableColumn id="6" xr3:uid="{A039C426-5E1C-496E-9BA3-741F605F2B65}" name="TP"/>
     <tableColumn id="7" xr3:uid="{A1835D25-C357-48CA-B5D0-E8E4A34199AD}" name="Accuracy2"/>
     <tableColumn id="8" xr3:uid="{56C8A5AF-FC9A-45E7-B43B-36A76C13A22E}" name="MSE2"/>
-    <tableColumn id="23" xr3:uid="{031F4430-2BEC-4614-BC7C-33B911E050EC}" name="Efficiency2" dataDxfId="1">
+    <tableColumn id="23" xr3:uid="{031F4430-2BEC-4614-BC7C-33B911E050EC}" name="Efficiency2" dataDxfId="4">
       <calculatedColumnFormula>(Table2[[#This Row],[TP2]]/(Table2[[#This Row],[TP2]]+Table2[[#This Row],[FN2]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{D8499300-B403-4302-8E33-88BFD8A2F864}" name="TN2"/>
@@ -3310,7 +3352,7 @@
     <tableColumn id="12" xr3:uid="{AD9EEA69-4AB6-41B3-89D3-6B253D34A6C3}" name="TP2"/>
     <tableColumn id="19" xr3:uid="{7EDEBBA8-BEF5-40C1-9D93-A2D0D842EB7E}" name="Accuracy3"/>
     <tableColumn id="21" xr3:uid="{2E8FE1DB-67A4-4E82-8BAA-5FDD6838E39B}" name="MSE3"/>
-    <tableColumn id="24" xr3:uid="{F1724ABC-6B8C-4FBE-AF66-0E2CF70CA37A}" name="Efficiency3" dataDxfId="0">
+    <tableColumn id="24" xr3:uid="{F1724ABC-6B8C-4FBE-AF66-0E2CF70CA37A}" name="Efficiency3" dataDxfId="3">
       <calculatedColumnFormula>(Table2[[#This Row],[TP3]]/(Table2[[#This Row],[TP3]]+Table2[[#This Row],[FN3]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{06C849E0-9616-4742-9323-944F8092A1A8}" name="TN3"/>
@@ -3648,10 +3690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C1DA7B-14B3-4B4E-8744-FCF5DDA7F499}">
-  <dimension ref="B1:AF46"/>
+  <dimension ref="B1:AF93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -8003,10 +8045,397 @@
         <v>5.5302818512211797E-2</v>
       </c>
     </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="e">
+        <f>C4-J4</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" t="e">
+        <f t="shared" ref="C52:C93" si="0">C5-J5</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>8.1633536875839185E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>8.2932799999999585E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>6.431077043004052E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>6.3661166688310233E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>4.8503746048249585E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>4.4822658178509389E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>2.4901476765839536E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>-6.712571997748995E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>-1.8448746264778992E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>-8.683036680958045E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>-8.228314061755948E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>-8.3582348100990078E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>-8.3582348100990078E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>-8.3582348100990078E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>-8.3582348100990078E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>-8.3582348100990078E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>-7.7302845264379805E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="0"/>
+        <v>-7.3838291975220072E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>-7.9684725650680521E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="0"/>
+        <v>-1.9747953748212921E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="0"/>
+        <v>-7.6220172361519678E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="0"/>
+        <v>-2.9145554545060959E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="0"/>
+        <v>-1.4442856524186976E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="0"/>
+        <v>-1.7214499155515983E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="0"/>
+        <v>-3.9842362825339706E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="0"/>
+        <v>-5.079901260231301E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="0"/>
+        <v>-2.3970378069378073E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="0"/>
+        <v>-2.4446754146636995E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="0"/>
+        <v>-2.4446754146636995E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="0"/>
+        <v>-4.1358104889349656E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="0"/>
+        <v>2.2476289463426946E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="0"/>
+        <v>-5.2423021956606974E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="0"/>
+        <v>-0.20893421679442203</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="0"/>
+        <v>5.8464336754604496E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C1048576 J1:J1048576 Q1:Q1048576">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="J1:J1048576 Q1:Q1048576 C1:C1048576">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8018,7 +8447,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C46">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8030,6 +8459,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 L1:L1048576 S1:S1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:X46">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC4:AC46">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -8041,19 +8506,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X4:X46">
+  <conditionalFormatting sqref="AE4:AE46">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -8065,28 +8518,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC4:AC46">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
+  <conditionalFormatting sqref="C51:C93">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE4:AE46">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>